<commit_message>
Debugged arnot to 3ish decimals
</commit_message>
<xml_diff>
--- a/sheets/input/Arnot_match.xlsx
+++ b/sheets/input/Arnot_match.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="0" windowWidth="19500" windowHeight="17540" tabRatio="790" activeTab="3"/>
+    <workbookView xWindow="1360" yWindow="0" windowWidth="20320" windowHeight="28340" tabRatio="790" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" r:id="rId1"/>
@@ -385,19 +385,19 @@
     <t>Gammarus</t>
   </si>
   <si>
-    <t>Lipid organic matter to water octonal proptionality constant (default = 1)</t>
-  </si>
-  <si>
-    <t>Non-Lipid organic matter to water octonal proptionality constant (default = .35)</t>
-  </si>
-  <si>
-    <t>Lipid organic matter in gut to biota octonal proptionality constant (default = 1)</t>
-  </si>
-  <si>
-    <t>Non-Lipid organic Carbon in gut to biota octonal proptionality constant (default = .35)</t>
-  </si>
-  <si>
-    <t>Non-Lipid organic matter in gut to biotaoctonal proptionality constant (defualt = .035)</t>
+    <t xml:space="preserve"> Beta Lipid Omn (default = 1)</t>
+  </si>
+  <si>
+    <t>Beta Non-lipid OM (defualt = 0.035)</t>
+  </si>
+  <si>
+    <t>Beta Lipid digesta (default = 1)</t>
+  </si>
+  <si>
+    <t>Beta Sediment OC (default = .35)</t>
+  </si>
+  <si>
+    <t>Beta  Non-lipid digesta  (defualt = .035)</t>
   </si>
 </sst>
 </file>
@@ -2127,8 +2127,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11430000" y="279400"/>
-          <a:ext cx="736600" cy="2057400"/>
+          <a:off x="11438467" y="279400"/>
+          <a:ext cx="736600" cy="2091267"/>
           <a:chOff x="11430000" y="279400"/>
           <a:chExt cx="736600" cy="2019300"/>
         </a:xfrm>
@@ -2759,8 +2759,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12611100" y="1866900"/>
-          <a:ext cx="825500" cy="889000"/>
+          <a:off x="12619567" y="1905000"/>
+          <a:ext cx="829733" cy="905933"/>
           <a:chOff x="11582400" y="182218"/>
           <a:chExt cx="2171700" cy="579782"/>
         </a:xfrm>
@@ -2882,8 +2882,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12573000" y="101600"/>
-          <a:ext cx="4127500" cy="3086100"/>
+          <a:off x="12581467" y="101600"/>
+          <a:ext cx="4148666" cy="3149600"/>
           <a:chOff x="11582400" y="190500"/>
           <a:chExt cx="1409700" cy="571500"/>
         </a:xfrm>
@@ -4704,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -5167,8 +5167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5514,8 +5514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5691,7 +5691,9 @@
       <c r="D6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <v>0.05</v>
+      </c>
       <c r="F6" s="26"/>
       <c r="G6" s="23" t="s">
         <v>28</v>
@@ -5897,7 +5899,9 @@
       <c r="D18" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>0.05</v>
+      </c>
       <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:6">
@@ -5987,7 +5991,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added convergance test, fixed prey con bug
</commit_message>
<xml_diff>
--- a/sheets/input/Arnot_match.xlsx
+++ b/sheets/input/Arnot_match.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sample and Time Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="Organism Diet" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Migratory Input" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Sample Sites" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -57,13 +58,13 @@
     <t xml:space="preserve">Ending Date</t>
   </si>
   <si>
-    <t xml:space="preserve">1,3,2012</t>
+    <t xml:space="preserve">1,1,2013</t>
   </si>
   <si>
     <t xml:space="preserve">Step</t>
   </si>
   <si>
-    <t xml:space="preserve">Days</t>
+    <t xml:space="preserve">Weeks</t>
   </si>
   <si>
     <t xml:space="preserve">Solving Options</t>
@@ -251,7 +252,7 @@
     <t xml:space="preserve">Dissolved Concentration in Water (ug/L) </t>
   </si>
   <si>
-    <t xml:space="preserve">Concentration in Pore Water (ug/L)</t>
+    <t xml:space="preserve">Concentration in Pore Water (ug/L) </t>
   </si>
   <si>
     <t xml:space="preserve">Fish</t>
@@ -326,13 +327,10 @@
     <t xml:space="preserve">Abundance (time step 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Fish 1 (replace with name)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boundary:</t>
   </si>
   <si>
-    <t xml:space="preserve">Coordinate 1 (x,y) (meters)</t>
+    <t xml:space="preserve">Coordinate 1 (x, y) (meters)</t>
   </si>
   <si>
     <t xml:space="preserve">Coordinate 2</t>
@@ -344,16 +342,16 @@
     <t xml:space="preserve">Coordinate 4</t>
   </si>
   <si>
-    <t xml:space="preserve">0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,0</t>
+    <t xml:space="preserve">0, 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30, 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30, 0</t>
   </si>
   <si>
     <t xml:space="preserve">Sites:</t>
@@ -362,10 +360,10 @@
     <t xml:space="preserve">Site Name</t>
   </si>
   <si>
-    <t xml:space="preserve">(x,y) (meters)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,10</t>
+    <t xml:space="preserve">(x, y) (meters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 10</t>
   </si>
   <si>
     <t xml:space="preserve">Number of Regional Samples per Fish Population :</t>
@@ -399,12 +397,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attraction Factor 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,0</t>
   </si>
 </sst>
 </file>
@@ -416,7 +408,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -544,7 +536,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -554,8 +546,14 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,6 +618,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -951,23 +955,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1007,11 +1011,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,7 +1031,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1035,11 +1039,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1047,15 +1051,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,7 +1116,7 @@
       <rgbColor rgb="FFFAC090"/>
       <rgbColor rgb="FF538DD5"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -1142,9 +1146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1019160</xdr:colOff>
+      <xdr:colOff>1018440</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1154,7 +1158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14044680" y="863280"/>
-          <a:ext cx="9471600" cy="7619400"/>
+          <a:ext cx="9470880" cy="7618680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1621,9 +1625,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3631320</xdr:colOff>
+      <xdr:colOff>3630600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>182160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1633,7 +1637,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12356640" y="699480"/>
-          <a:ext cx="3084840" cy="995760"/>
+          <a:ext cx="3084120" cy="995040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1844,9 +1848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2331720</xdr:colOff>
+      <xdr:colOff>2331000</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1860,7 +1864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16507800" y="10278720"/>
-          <a:ext cx="2331720" cy="735840"/>
+          <a:ext cx="2331000" cy="735120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1881,9 +1885,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4761000</xdr:colOff>
+      <xdr:colOff>4760280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1893,7 +1897,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11824920" y="2007000"/>
-          <a:ext cx="9443880" cy="3201480"/>
+          <a:ext cx="9443160" cy="3200760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2353,16 +2357,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>356040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1623960</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>786600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:colOff>255600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2371,8 +2375,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16928640" y="190440"/>
-          <a:ext cx="3603600" cy="761400"/>
+          <a:off x="16398360" y="1476360"/>
+          <a:ext cx="3602880" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2502,9 +2506,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
+      <xdr:colOff>1132560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2514,7 +2518,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14774760" y="1714680"/>
-          <a:ext cx="2931120" cy="761040"/>
+          <a:ext cx="2930400" cy="760320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2572,6 +2576,681 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>167040</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>568440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="28071360" y="190440"/>
+          <a:ext cx="1421280" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>176400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>581400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="39267360" y="190440"/>
+          <a:ext cx="1424880" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>176400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>581400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="50485320" y="190440"/>
+          <a:ext cx="1424880" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>552600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>84960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="69218280" y="190440"/>
+          <a:ext cx="1571760" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>960120</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>162720</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="80843400" y="190440"/>
+          <a:ext cx="1242360" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>550080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>776160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="90631800" y="190440"/>
+          <a:ext cx="1245600" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>90</xdr:col>
+      <xdr:colOff>159840</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>385920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="100439640" y="190440"/>
+          <a:ext cx="1245600" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>107</xdr:col>
+      <xdr:colOff>552600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>109</xdr:col>
+      <xdr:colOff>84600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="118168920" y="190440"/>
+          <a:ext cx="1571760" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>118</xdr:col>
+      <xdr:colOff>959760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>120</xdr:col>
+      <xdr:colOff>162720</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="129794040" y="190440"/>
+          <a:ext cx="1242720" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>128</xdr:col>
+      <xdr:colOff>550440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>129</xdr:col>
+      <xdr:colOff>776160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="139582800" y="190440"/>
+          <a:ext cx="1245600" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>138</xdr:col>
+      <xdr:colOff>159840</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>139</xdr:col>
+      <xdr:colOff>385920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="149390280" y="190440"/>
+          <a:ext cx="1245960" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>155</xdr:col>
+      <xdr:colOff>552600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>157</xdr:col>
+      <xdr:colOff>84600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="167119920" y="190440"/>
+          <a:ext cx="1571760" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>166</xdr:col>
+      <xdr:colOff>959760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>168</xdr:col>
+      <xdr:colOff>163080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="178745040" y="190440"/>
+          <a:ext cx="1242720" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>176</xdr:col>
+      <xdr:colOff>550440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>177</xdr:col>
+      <xdr:colOff>776160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="188533800" y="190440"/>
+          <a:ext cx="1245600" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>186</xdr:col>
+      <xdr:colOff>159840</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>187</xdr:col>
+      <xdr:colOff>385920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="198341280" y="190440"/>
+          <a:ext cx="1245960" cy="360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2586,19 +3265,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>643680</xdr:colOff>
+      <xdr:colOff>642960</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvPr id="28" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8870760" y="2521800"/>
-          <a:ext cx="9088560" cy="3568320"/>
+          <a:ext cx="9087840" cy="3567600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3126,19 +3805,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>151560</xdr:colOff>
+      <xdr:colOff>150840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvPr id="29" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8939880" y="674280"/>
-          <a:ext cx="4075920" cy="949680"/>
+          <a:ext cx="4075200" cy="948960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3206,7 +3885,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Line 1"/>
+        <xdr:cNvPr id="30" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3245,19 +3924,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3566880</xdr:colOff>
+      <xdr:colOff>3566160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvPr id="31" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4629240" y="4925160"/>
-          <a:ext cx="5158440" cy="761400"/>
+          <a:ext cx="5157720" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3320,7 +3999,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Line 1"/>
+        <xdr:cNvPr id="32" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3359,19 +4038,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2593440</xdr:colOff>
+      <xdr:colOff>2592720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvPr id="33" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16049880" y="5488560"/>
-          <a:ext cx="4331520" cy="341640"/>
+          <a:ext cx="4330800" cy="340920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3443,19 +4122,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5384160</xdr:colOff>
+      <xdr:colOff>5383440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="CustomShape 1"/>
+        <xdr:cNvPr id="34" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5257080" cy="1497600"/>
+          <a:ext cx="5256360" cy="1496880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3528,7 +4207,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Line 1"/>
+        <xdr:cNvPr id="35" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3573,7 +4252,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Line 1"/>
+        <xdr:cNvPr id="36" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3618,7 +4297,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Line 1"/>
+        <xdr:cNvPr id="37" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3657,19 +4336,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6884640</xdr:colOff>
+      <xdr:colOff>6883920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="CustomShape 1"/>
+        <xdr:cNvPr id="38" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10153440" y="2298600"/>
-          <a:ext cx="5817960" cy="659520"/>
+          <a:ext cx="5817240" cy="658800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3737,7 +4416,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Line 1"/>
+        <xdr:cNvPr id="39" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3776,19 +4455,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="CustomShape 1"/>
+        <xdr:cNvPr id="40" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11960640" y="241200"/>
-          <a:ext cx="5136480" cy="392760"/>
+          <a:ext cx="5135760" cy="392040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3861,7 +4540,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Line 1"/>
+        <xdr:cNvPr id="41" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3900,19 +4579,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="CustomShape 1"/>
+        <xdr:cNvPr id="42" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12062160" y="1295280"/>
-          <a:ext cx="3862800" cy="418320"/>
+          <a:ext cx="3862080" cy="417600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3969,19 +4648,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>469440</xdr:colOff>
+      <xdr:colOff>468720</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="CustomShape 1"/>
+        <xdr:cNvPr id="43" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12087720" y="2158560"/>
-          <a:ext cx="5225400" cy="698040"/>
+          <a:ext cx="5224680" cy="697320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4029,6 +4708,401 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>620280</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>644760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="36809280" y="241200"/>
+          <a:ext cx="4104000" cy="392040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Copy and Paste Column to the right for more times.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>466200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>949680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="59091120" y="241200"/>
+          <a:ext cx="4562640" cy="392040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Copy and Paste Column to the right for more times.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>104760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>76</xdr:col>
+      <xdr:colOff>691560</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="81165600" y="241200"/>
+          <a:ext cx="3646080" cy="392040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Copy and Paste Column to the right for more times.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>93</xdr:col>
+      <xdr:colOff>465840</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>97</xdr:col>
+      <xdr:colOff>949320</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="101922840" y="241200"/>
+          <a:ext cx="4562640" cy="392040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Copy and Paste Column to the right for more times.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>115</xdr:col>
+      <xdr:colOff>104760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>118</xdr:col>
+      <xdr:colOff>691560</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123997680" y="241200"/>
+          <a:ext cx="3646080" cy="392040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="ffffff"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Copy and Paste Column to the right for more times.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4043,19 +5117,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>278640</xdr:colOff>
+      <xdr:colOff>277920</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="CustomShape 1"/>
+        <xdr:cNvPr id="49" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6531120" cy="5879520"/>
+          <a:ext cx="6530400" cy="5878800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4172,7 +5246,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4284,6 +5358,32 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.36"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -4292,7 +5392,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4616,10 +5716,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:GK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="EJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="EP2" activeCellId="0" sqref="EP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4668,6 +5768,573 @@
       <c r="D2" s="1" t="n">
         <v>13</v>
       </c>
+      <c r="E2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="F2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="H2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="K2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="L2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="N2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="O2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="S2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="T2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="V2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="W2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AB2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AG2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AI2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AJ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AK2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AM2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AO2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AP2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AQ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AR2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AT2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AV2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AW2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AX2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="AY2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="AZ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BA2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BB2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BC2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BD2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BE2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BF2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BG2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BH2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BI2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BJ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BK2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BL2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BM2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BN2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BO2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BP2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BQ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BR2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BS2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BT2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BU2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="BV2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BW2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BX2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="BY2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="BZ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CA2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CB2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CC2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CD2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CE2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CF2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CG2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CH2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CI2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CJ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CK2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CL2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CM2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CN2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CO2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CP2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CQ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CR2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CS2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CT2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CU2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CV2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CW2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="CX2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="CY2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="CZ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DA2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DB2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DC2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DD2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DE2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DF2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DG2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DH2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DI2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DJ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DK2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DL2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DM2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DN2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DO2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DP2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DQ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DR2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DS2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DT2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DU2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DV2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DW2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="DX2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="DY2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="DZ2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EA2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EB2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EC2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="ED2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EE2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EF2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EG2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EH2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EI2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EJ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EK2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EL2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EM2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EN2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EO2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EP2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EQ2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="ER2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="ES2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="ET2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EU2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EV2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EW2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="EX2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="EY2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="EZ2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FA2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FB2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FC2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FD2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FE2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FF2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FG2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FH2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FI2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FJ2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FK2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FL2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FM2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FN2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FO2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FP2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FQ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FR2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FS2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FT2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FU2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FV2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FW2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="FX2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="FY2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="FZ2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="GA2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="GB2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="GC2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="GD2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="GE2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="GF2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="GG2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="GH2" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="GI2" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="GJ2" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="GK2" s="1" t="n">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4688,8 +6355,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4760,41 +6427,31 @@
       <c r="A6" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="32" t="n">
-        <v>1</v>
-      </c>
+      <c r="B6" s="32"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="33" t="n">
-        <v>0.35</v>
-      </c>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="32" t="n">
-        <v>1</v>
-      </c>
+      <c r="B8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="32" t="n">
-        <v>0.35</v>
-      </c>
+      <c r="B9" s="32"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="36" t="n">
-        <v>0.035</v>
-      </c>
+      <c r="B10" s="36"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -4859,10 +6516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:GK7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="EG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="EP4" activeCellId="0" sqref="EP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4887,31 +6544,1182 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>3.881</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="Y4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="Z4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AR4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AS4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AT4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="AZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BR4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BS4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BT4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="BZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CR4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CS4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CT4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="CZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DR4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DS4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DT4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="DZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="ED4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="ER4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="ES4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="ET4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="EZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FL4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FM4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FN4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FO4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FP4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FQ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FR4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FS4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FT4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FU4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FV4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FW4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FX4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FY4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="FZ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GA4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GB4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GC4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GD4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GE4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GF4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GG4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GH4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GI4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GJ4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+      <c r="GK4" s="3" t="n">
+        <v>3.881</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>0.028</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="B5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="S5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="U5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="V5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="X5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="Y5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="Z5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AR5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AS5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AT5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="AZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BR5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BS5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BT5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="BZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CR5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CS5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CT5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="CZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DR5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DS5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DT5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="DZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="ED5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="ER5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="ES5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="ET5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="EZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FL5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FM5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FN5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FO5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FP5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FQ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FR5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FS5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FT5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FU5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FV5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FW5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FX5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FY5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="FZ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GA5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GB5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GC5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GD5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GE5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GF5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GG5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GH5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GI5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GJ5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="GK5" s="3" t="n">
+        <v>0.028</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="42"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="B6" s="43"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="43"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4931,8 +7739,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5006,7 +7814,7 @@
         <v>74</v>
       </c>
       <c r="B3" s="48" t="n">
-        <v>0.0004</v>
+        <v>0.034</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>74</v>
@@ -5032,7 +7840,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="12" t="n">
-        <v>0.021</v>
+        <v>0.025</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>76</v>
@@ -5318,7 +8126,7 @@
   </sheetPr>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -5566,8 +8374,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="DN9" activeCellId="0" sqref="DN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6091,7 +8899,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B2" s="62" t="n">
         <v>1</v>
@@ -6100,6 +8908,375 @@
         <v>1</v>
       </c>
       <c r="D2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CO2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CS2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DA2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DB2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DE2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DJ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DL2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DM2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DO2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DQ2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DR2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DS2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DT2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DU2" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV2" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="DW2" s="63" t="n">
         <v>1</v>
       </c>
       <c r="FU2" s="31"/>
@@ -6140,8 +9317,8 @@
   </sheetPr>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6158,19 +9335,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
@@ -6179,16 +9356,16 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
@@ -6196,13 +9373,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D3" s="31"/>
       <c r="E3" s="31"/>
@@ -6216,7 +9393,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -6566,16 +9743,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B39" s="65" t="n">
         <v>40</v>
       </c>
       <c r="C39" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="65" t="s">
         <v>107</v>
-      </c>
-      <c r="D39" s="65" t="s">
-        <v>108</v>
       </c>
       <c r="E39" s="31"/>
       <c r="F39" s="31"/>
@@ -6584,49 +9761,49 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="62" t="s">
+      <c r="C40" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="62" t="s">
+      <c r="D40" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="E40" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="66" t="s">
+      <c r="F40" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="66" t="s">
+      <c r="G40" s="66" t="s">
         <v>114</v>
-      </c>
-      <c r="G40" s="66" t="s">
-        <v>115</v>
       </c>
       <c r="H40" s="67"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="62" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C41" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="D41" s="62" t="s">
+      <c r="D41" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="F41" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="G41" s="62" t="s">
-        <v>118</v>
+      <c r="F41" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="H41" s="31"/>
       <c r="AW41" s="0" t="s">

</xml_diff>